<commit_message>
Pushing all changes to the WIAA Webscrape project.
</commit_message>
<xml_diff>
--- a/wiaaWebscrape/misses.xlsx
+++ b/wiaaWebscrape/misses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="123">
   <si>
     <t>Team</t>
   </si>
@@ -55,6 +55,12 @@
     <t>Error</t>
   </si>
   <si>
+    <t>Neenah</t>
+  </si>
+  <si>
+    <t>Eau Claire Memorial</t>
+  </si>
+  <si>
     <t>Stevens Point</t>
   </si>
   <si>
@@ -133,18 +139,18 @@
     <t>Milwaukee Madison</t>
   </si>
   <si>
-    <t>Jefferson</t>
-  </si>
-  <si>
-    <t>Milton</t>
-  </si>
-  <si>
     <t>Pius XI Catholic</t>
   </si>
   <si>
     <t>Whitefish Bay</t>
   </si>
   <si>
+    <t>Waterford</t>
+  </si>
+  <si>
+    <t>Cudahy</t>
+  </si>
+  <si>
     <t>Somerset</t>
   </si>
   <si>
@@ -196,12 +202,6 @@
     <t>North Fond du Lac</t>
   </si>
   <si>
-    <t>Golda Meir</t>
-  </si>
-  <si>
-    <t>Messmer</t>
-  </si>
-  <si>
     <t>Grantsburg</t>
   </si>
   <si>
@@ -247,6 +247,12 @@
     <t>Horicon</t>
   </si>
   <si>
+    <t>Eau Claire Immanuel Lutheran</t>
+  </si>
+  <si>
+    <t>Prairie Farm</t>
+  </si>
+  <si>
     <t>Northwood</t>
   </si>
   <si>
@@ -265,15 +271,15 @@
     <t>Gilman</t>
   </si>
   <si>
-    <t>Washburn</t>
-  </si>
-  <si>
     <t>Flambeau</t>
   </si>
   <si>
     <t>Mercer</t>
   </si>
   <si>
+    <t>Rib Lake</t>
+  </si>
+  <si>
     <t>Newman Catholic</t>
   </si>
   <si>
@@ -289,12 +295,6 @@
     <t>Suring</t>
   </si>
   <si>
-    <t>Independence/Gilmanton</t>
-  </si>
-  <si>
-    <t>Cashton</t>
-  </si>
-  <si>
     <t>Blair-Taylor</t>
   </si>
   <si>
@@ -304,6 +304,9 @@
     <t>Wauzeka-Steuben</t>
   </si>
   <si>
+    <t>Belmont</t>
+  </si>
+  <si>
     <t>Highland</t>
   </si>
   <si>
@@ -331,6 +334,12 @@
     <t>Southwestern</t>
   </si>
   <si>
+    <t>Fall River</t>
+  </si>
+  <si>
+    <t>Central WI Christian</t>
+  </si>
+  <si>
     <t>Cambria-Friesland</t>
   </si>
   <si>
@@ -343,6 +352,9 @@
     <t>Chesterton Academy</t>
   </si>
   <si>
+    <t>Palmyra-Eagle</t>
+  </si>
+  <si>
     <t>Kenosha Christian Life</t>
   </si>
   <si>
@@ -361,16 +373,16 @@
     <t>2B</t>
   </si>
   <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
     <t>3B</t>
-  </si>
-  <si>
-    <t>1B</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t>4B</t>
   </si>
 </sst>
 </file>
@@ -728,7 +740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M99"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -783,34 +795,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>2024</v>
       </c>
       <c r="F2">
-        <v>0.681818</v>
+        <v>0.826087</v>
       </c>
       <c r="G2">
-        <v>0.470954</v>
+        <v>0.535714</v>
       </c>
       <c r="H2">
-        <v>0.528058</v>
+        <v>0.560331</v>
       </c>
       <c r="I2">
-        <v>0.435583</v>
+        <v>0.470024</v>
       </c>
       <c r="J2">
-        <v>0.505771</v>
+        <v>0.553137</v>
       </c>
       <c r="K2">
-        <v>0.543770692016896</v>
+        <v>0.6350098271660964</v>
       </c>
       <c r="L2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -824,34 +836,34 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>2024</v>
       </c>
       <c r="F3">
-        <v>0.619048</v>
+        <v>0.863636</v>
       </c>
       <c r="G3">
-        <v>0.538071</v>
+        <v>0.508163</v>
       </c>
       <c r="H3">
-        <v>0.525766</v>
+        <v>0.540215</v>
       </c>
       <c r="I3">
-        <v>0.504348</v>
+        <v>0.460993</v>
       </c>
       <c r="J3">
-        <v>0.5115459999999999</v>
+        <v>0.53204</v>
       </c>
       <c r="K3">
-        <v>0.5549944003274239</v>
+        <v>0.6357708632979633</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -865,34 +877,34 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>2024</v>
       </c>
       <c r="F4">
-        <v>0.52381</v>
+        <v>0.681818</v>
       </c>
       <c r="G4">
-        <v>0.568376</v>
+        <v>0.470954</v>
       </c>
       <c r="H4">
-        <v>0.530409</v>
+        <v>0.528058</v>
       </c>
       <c r="I4">
-        <v>0.390244</v>
+        <v>0.435583</v>
       </c>
       <c r="J4">
-        <v>0.541032</v>
+        <v>0.505771</v>
       </c>
       <c r="K4">
-        <v>0.5173253409625973</v>
+        <v>0.5477260665482666</v>
       </c>
       <c r="L4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -906,34 +918,34 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>2024</v>
       </c>
       <c r="F5">
-        <v>0.565217</v>
+        <v>0.619048</v>
       </c>
       <c r="G5">
-        <v>0.530815</v>
+        <v>0.538071</v>
       </c>
       <c r="H5">
-        <v>0.54705</v>
+        <v>0.525766</v>
       </c>
       <c r="I5">
-        <v>0.392982</v>
+        <v>0.504348</v>
       </c>
       <c r="J5">
-        <v>0.530579</v>
+        <v>0.5115459999999999</v>
       </c>
       <c r="K5">
-        <v>0.5196689967636319</v>
+        <v>0.5600761055072477</v>
       </c>
       <c r="L5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -947,34 +959,34 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>2024</v>
       </c>
       <c r="F6">
-        <v>0.428571</v>
+        <v>0.52381</v>
       </c>
       <c r="G6">
-        <v>0.513978</v>
+        <v>0.568376</v>
       </c>
       <c r="H6">
-        <v>0.5096079999999999</v>
+        <v>0.530409</v>
       </c>
       <c r="I6">
-        <v>0.319797</v>
+        <v>0.390244</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.541032</v>
       </c>
       <c r="K6">
-        <v>0.4499271792570497</v>
+        <v>0.5176422665120267</v>
       </c>
       <c r="L6">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -988,34 +1000,34 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>2024</v>
       </c>
       <c r="F7">
-        <v>0.363636</v>
+        <v>0.565217</v>
       </c>
       <c r="G7">
-        <v>0.574786</v>
+        <v>0.530815</v>
       </c>
       <c r="H7">
-        <v>0.533094</v>
+        <v>0.54705</v>
       </c>
       <c r="I7">
-        <v>0.377358</v>
+        <v>0.392982</v>
       </c>
       <c r="J7">
-        <v>0.516358</v>
+        <v>0.530579</v>
       </c>
       <c r="K7">
-        <v>0.4593700449043512</v>
+        <v>0.5198929955333654</v>
       </c>
       <c r="L7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1029,34 +1041,34 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>2024</v>
       </c>
       <c r="F8">
-        <v>0.863636</v>
+        <v>0.428571</v>
       </c>
       <c r="G8">
-        <v>0.541922</v>
+        <v>0.513978</v>
       </c>
       <c r="H8">
-        <v>0.544919</v>
+        <v>0.5096079999999999</v>
       </c>
       <c r="I8">
-        <v>0.490521</v>
+        <v>0.319797</v>
       </c>
       <c r="J8">
-        <v>0.545907</v>
+        <v>0.5</v>
       </c>
       <c r="K8">
-        <v>0.6423112141490591</v>
+        <v>0.4467987515316872</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1070,34 +1082,34 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>2024</v>
       </c>
       <c r="F9">
-        <v>0.909091</v>
+        <v>0.363636</v>
       </c>
       <c r="G9">
-        <v>0.5031060000000001</v>
+        <v>0.574786</v>
       </c>
       <c r="H9">
-        <v>0.556118</v>
+        <v>0.533094</v>
       </c>
       <c r="I9">
-        <v>0.474886</v>
+        <v>0.377358</v>
       </c>
       <c r="J9">
-        <v>0.552197</v>
+        <v>0.516358</v>
       </c>
       <c r="K9">
-        <v>0.6449035384179976</v>
+        <v>0.4554886023182455</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -1111,37 +1123,37 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>2024</v>
       </c>
       <c r="F10">
-        <v>0.304348</v>
+        <v>0.863636</v>
       </c>
       <c r="G10">
-        <v>0.478599</v>
+        <v>0.541922</v>
       </c>
       <c r="H10">
-        <v>0.497454</v>
+        <v>0.544919</v>
       </c>
       <c r="I10">
-        <v>0.282051</v>
+        <v>0.490521</v>
       </c>
       <c r="J10">
-        <v>0.507728</v>
+        <v>0.545907</v>
       </c>
       <c r="K10">
-        <v>0.391885603613533</v>
+        <v>0.6539725221156059</v>
       </c>
       <c r="L10">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1152,34 +1164,34 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>2024</v>
       </c>
       <c r="F11">
-        <v>0.272727</v>
+        <v>0.909091</v>
       </c>
       <c r="G11">
-        <v>0.524291</v>
+        <v>0.5031060000000001</v>
       </c>
       <c r="H11">
-        <v>0.49644</v>
+        <v>0.556118</v>
       </c>
       <c r="I11">
-        <v>0.242647</v>
+        <v>0.474886</v>
       </c>
       <c r="J11">
-        <v>0.501965</v>
+        <v>0.552197</v>
       </c>
       <c r="K11">
-        <v>0.3871651342626606</v>
+        <v>0.6554548215457401</v>
       </c>
       <c r="L11">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -1193,37 +1205,37 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>2024</v>
       </c>
       <c r="F12">
-        <v>0.136364</v>
+        <v>0.304348</v>
       </c>
       <c r="G12">
-        <v>0.6367429999999999</v>
+        <v>0.478599</v>
       </c>
       <c r="H12">
-        <v>0.542874</v>
+        <v>0.497454</v>
       </c>
       <c r="I12">
-        <v>0.370968</v>
+        <v>0.282051</v>
       </c>
       <c r="J12">
-        <v>0.530474</v>
+        <v>0.507728</v>
       </c>
       <c r="K12">
-        <v>0.4027087874055214</v>
+        <v>0.3817633751297706</v>
       </c>
       <c r="L12">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1234,34 +1246,34 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E13">
         <v>2024</v>
       </c>
       <c r="F13">
-        <v>0.722222</v>
+        <v>0.272727</v>
       </c>
       <c r="G13">
-        <v>0.391192</v>
+        <v>0.524291</v>
       </c>
       <c r="H13">
-        <v>0.453023</v>
+        <v>0.49644</v>
       </c>
       <c r="I13">
-        <v>0.330909</v>
+        <v>0.242647</v>
       </c>
       <c r="J13">
-        <v>0.422107</v>
+        <v>0.501965</v>
       </c>
       <c r="K13">
-        <v>0.4998504655977207</v>
+        <v>0.3784664284049167</v>
       </c>
       <c r="L13">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1275,37 +1287,37 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <v>2024</v>
       </c>
       <c r="F14">
-        <v>0.8</v>
+        <v>0.136364</v>
       </c>
       <c r="G14">
-        <v>0.336538</v>
+        <v>0.6367429999999999</v>
       </c>
       <c r="H14">
-        <v>0.463713</v>
+        <v>0.542874</v>
       </c>
       <c r="I14">
-        <v>0.290984</v>
+        <v>0.370968</v>
       </c>
       <c r="J14">
-        <v>0.473054</v>
+        <v>0.530474</v>
       </c>
       <c r="K14">
-        <v>0.5114282379139198</v>
+        <v>0.3921457202184201</v>
       </c>
       <c r="L14">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1316,34 +1328,34 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>2024</v>
       </c>
       <c r="F15">
-        <v>0.454545</v>
+        <v>0.722222</v>
       </c>
       <c r="G15">
-        <v>0.483193</v>
+        <v>0.391192</v>
       </c>
       <c r="H15">
-        <v>0.513999</v>
+        <v>0.453023</v>
       </c>
       <c r="I15">
-        <v>0.32381</v>
+        <v>0.330909</v>
       </c>
       <c r="J15">
-        <v>0.485209</v>
+        <v>0.422107</v>
       </c>
       <c r="K15">
-        <v>0.4481132979972862</v>
+        <v>0.5084115640508945</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -1357,34 +1369,34 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16">
         <v>2024</v>
       </c>
       <c r="F16">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G16">
-        <v>0.46473</v>
+        <v>0.336538</v>
       </c>
       <c r="H16">
-        <v>0.510389</v>
+        <v>0.463713</v>
       </c>
       <c r="I16">
-        <v>0.285714</v>
+        <v>0.290984</v>
       </c>
       <c r="J16">
-        <v>0.51419</v>
+        <v>0.473054</v>
       </c>
       <c r="K16">
-        <v>0.455838267372057</v>
+        <v>0.5160848105514793</v>
       </c>
       <c r="L16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -1398,37 +1410,37 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D17">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>2024</v>
       </c>
       <c r="F17">
-        <v>0.26087</v>
+        <v>0.454545</v>
       </c>
       <c r="G17">
-        <v>0.371179</v>
+        <v>0.483193</v>
       </c>
       <c r="H17">
-        <v>0.436844</v>
+        <v>0.513999</v>
       </c>
       <c r="I17">
-        <v>0.242991</v>
+        <v>0.32381</v>
       </c>
       <c r="J17">
-        <v>0.434241</v>
+        <v>0.485209</v>
       </c>
       <c r="K17">
-        <v>0.3248192807222551</v>
+        <v>0.4452877743167108</v>
       </c>
       <c r="L17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1439,34 +1451,34 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D18">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>2024</v>
       </c>
       <c r="F18">
-        <v>0.181818</v>
+        <v>0.5</v>
       </c>
       <c r="G18">
-        <v>0.554167</v>
+        <v>0.46473</v>
       </c>
       <c r="H18">
-        <v>0.533314</v>
+        <v>0.510389</v>
       </c>
       <c r="I18">
-        <v>0.174419</v>
+        <v>0.285714</v>
       </c>
       <c r="J18">
-        <v>0.518499</v>
+        <v>0.51419</v>
       </c>
       <c r="K18">
-        <v>0.3579404411757974</v>
+        <v>0.4516798494944052</v>
       </c>
       <c r="L18">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1480,37 +1492,37 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19">
         <v>2024</v>
       </c>
       <c r="F19">
-        <v>0.047619</v>
+        <v>0.26087</v>
       </c>
       <c r="G19">
-        <v>0.495652</v>
+        <v>0.371179</v>
       </c>
       <c r="H19">
-        <v>0.513272</v>
+        <v>0.436844</v>
       </c>
       <c r="I19">
-        <v>0.26087</v>
+        <v>0.242991</v>
       </c>
       <c r="J19">
-        <v>0.371179</v>
+        <v>0.434241</v>
       </c>
       <c r="K19">
-        <v>0.2863308501125358</v>
+        <v>0.3138911945723494</v>
       </c>
       <c r="L19">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1521,37 +1533,37 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20">
         <v>2024</v>
       </c>
       <c r="F20">
-        <v>0.142857</v>
+        <v>0.181818</v>
       </c>
       <c r="G20">
-        <v>0.495671</v>
+        <v>0.554167</v>
       </c>
       <c r="H20">
-        <v>0.495417</v>
+        <v>0.533314</v>
       </c>
       <c r="I20">
-        <v>0.227273</v>
+        <v>0.174419</v>
       </c>
       <c r="J20">
-        <v>0.454545</v>
+        <v>0.518499</v>
       </c>
       <c r="K20">
-        <v>0.3249196535190655</v>
+        <v>0.3448928971201031</v>
       </c>
       <c r="L20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1562,37 +1574,37 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>2024</v>
+      </c>
+      <c r="F21">
+        <v>0.047619</v>
+      </c>
+      <c r="G21">
+        <v>0.495652</v>
+      </c>
+      <c r="H21">
+        <v>0.513272</v>
+      </c>
+      <c r="I21">
+        <v>0.26087</v>
+      </c>
+      <c r="J21">
+        <v>0.371179</v>
+      </c>
+      <c r="K21">
+        <v>0.2762418475491066</v>
+      </c>
+      <c r="L21">
         <v>17</v>
       </c>
-      <c r="E21">
-        <v>2024</v>
-      </c>
-      <c r="F21">
-        <v>0.136364</v>
-      </c>
-      <c r="G21">
-        <v>0.419069</v>
-      </c>
-      <c r="H21">
-        <v>0.438553</v>
-      </c>
-      <c r="I21">
-        <v>0.215385</v>
-      </c>
-      <c r="J21">
-        <v>0.411281</v>
-      </c>
-      <c r="K21">
-        <v>0.2889080533931762</v>
-      </c>
-      <c r="L21">
-        <v>16</v>
-      </c>
       <c r="M21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1600,37 +1612,37 @@
         <v>33</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E22">
         <v>2024</v>
       </c>
       <c r="F22">
-        <v>0.47619</v>
+        <v>0.142857</v>
       </c>
       <c r="G22">
-        <v>0.495633</v>
+        <v>0.495671</v>
       </c>
       <c r="H22">
-        <v>0.5047509999999999</v>
+        <v>0.495417</v>
       </c>
       <c r="I22">
-        <v>0.376147</v>
+        <v>0.227273</v>
       </c>
       <c r="J22">
-        <v>0.501706</v>
+        <v>0.454545</v>
       </c>
       <c r="K22">
-        <v>0.4701447050942457</v>
+        <v>0.3129995583402208</v>
       </c>
       <c r="L22">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -1641,37 +1653,37 @@
         <v>34</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E23">
         <v>2024</v>
       </c>
       <c r="F23">
-        <v>0.478261</v>
+        <v>0.136364</v>
       </c>
       <c r="G23">
-        <v>0.535714</v>
+        <v>0.419069</v>
       </c>
       <c r="H23">
-        <v>0.547611</v>
+        <v>0.438553</v>
       </c>
       <c r="I23">
-        <v>0.345833</v>
+        <v>0.215385</v>
       </c>
       <c r="J23">
-        <v>0.539095</v>
+        <v>0.411281</v>
       </c>
       <c r="K23">
-        <v>0.4851828525039115</v>
+        <v>0.277152991427227</v>
       </c>
       <c r="L23">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1685,34 +1697,34 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>2024</v>
+      </c>
+      <c r="F24">
+        <v>0.47619</v>
+      </c>
+      <c r="G24">
+        <v>0.495633</v>
+      </c>
+      <c r="H24">
+        <v>0.5047509999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.376147</v>
+      </c>
+      <c r="J24">
+        <v>0.501706</v>
+      </c>
+      <c r="K24">
+        <v>0.4681561885480752</v>
+      </c>
+      <c r="L24">
         <v>8</v>
-      </c>
-      <c r="E24">
-        <v>2024</v>
-      </c>
-      <c r="F24">
-        <v>0.333333</v>
-      </c>
-      <c r="G24">
-        <v>0.466523</v>
-      </c>
-      <c r="H24">
-        <v>0.528725</v>
-      </c>
-      <c r="I24">
-        <v>0.279221</v>
-      </c>
-      <c r="J24">
-        <v>0.502696</v>
-      </c>
-      <c r="K24">
-        <v>0.3981109926985682</v>
-      </c>
-      <c r="L24">
-        <v>9</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -1726,34 +1738,34 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25">
         <v>2024</v>
       </c>
       <c r="F25">
-        <v>0.347826</v>
+        <v>0.478261</v>
       </c>
       <c r="G25">
-        <v>0.496032</v>
+        <v>0.535714</v>
       </c>
       <c r="H25">
-        <v>0.52507</v>
+        <v>0.547611</v>
       </c>
       <c r="I25">
-        <v>0.282486</v>
+        <v>0.345833</v>
       </c>
       <c r="J25">
-        <v>0.528854</v>
+        <v>0.539095</v>
       </c>
       <c r="K25">
-        <v>0.4162071661035705</v>
+        <v>0.4815122404252992</v>
       </c>
       <c r="L25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -1767,7 +1779,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -1776,22 +1788,22 @@
         <v>2024</v>
       </c>
       <c r="F26">
-        <v>0.47619</v>
+        <v>0.333333</v>
       </c>
       <c r="G26">
-        <v>0.437642</v>
+        <v>0.466523</v>
       </c>
       <c r="H26">
-        <v>0.496215</v>
+        <v>0.528725</v>
       </c>
       <c r="I26">
-        <v>0.339806</v>
+        <v>0.279221</v>
       </c>
       <c r="J26">
-        <v>0.476025</v>
+        <v>0.502696</v>
       </c>
       <c r="K26">
-        <v>0.4424399291238778</v>
+        <v>0.3879718247533018</v>
       </c>
       <c r="L26">
         <v>9</v>
@@ -1808,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D27">
         <v>9</v>
@@ -1817,22 +1829,22 @@
         <v>2024</v>
       </c>
       <c r="F27">
-        <v>0.555556</v>
+        <v>0.347826</v>
       </c>
       <c r="G27">
-        <v>0.430962</v>
+        <v>0.496032</v>
       </c>
       <c r="H27">
-        <v>0.442712</v>
+        <v>0.52507</v>
       </c>
       <c r="I27">
-        <v>0.224299</v>
+        <v>0.282486</v>
       </c>
       <c r="J27">
-        <v>0.483871</v>
+        <v>0.528854</v>
       </c>
       <c r="K27">
-        <v>0.4465890627315767</v>
+        <v>0.4064711277243898</v>
       </c>
       <c r="L27">
         <v>8</v>
@@ -1849,34 +1861,34 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E28">
         <v>2024</v>
       </c>
       <c r="F28">
-        <v>0.5</v>
+        <v>0.47619</v>
       </c>
       <c r="G28">
-        <v>0.486653</v>
+        <v>0.437642</v>
       </c>
       <c r="H28">
-        <v>0.491413</v>
+        <v>0.496215</v>
       </c>
       <c r="I28">
-        <v>0.381148</v>
+        <v>0.339806</v>
       </c>
       <c r="J28">
-        <v>0.497326</v>
+        <v>0.476025</v>
       </c>
       <c r="K28">
-        <v>0.4751127734244949</v>
+        <v>0.4392318971202713</v>
       </c>
       <c r="L28">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -1890,34 +1902,34 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <v>2024</v>
       </c>
       <c r="F29">
-        <v>0.478261</v>
+        <v>0.555556</v>
       </c>
       <c r="G29">
-        <v>0.533203</v>
+        <v>0.430962</v>
       </c>
       <c r="H29">
-        <v>0.556165</v>
+        <v>0.442712</v>
       </c>
       <c r="I29">
-        <v>0.312757</v>
+        <v>0.224299</v>
       </c>
       <c r="J29">
-        <v>0.514025</v>
+        <v>0.483871</v>
       </c>
       <c r="K29">
-        <v>0.4752925239139296</v>
+        <v>0.4463548907637875</v>
       </c>
       <c r="L29">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -1931,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1955,7 +1967,7 @@
         <v>0.513894</v>
       </c>
       <c r="K30">
-        <v>0.5879671935800679</v>
+        <v>0.5975018834592668</v>
       </c>
       <c r="L30">
         <v>3</v>
@@ -1972,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1996,7 +2008,7 @@
         <v>0.542745</v>
       </c>
       <c r="K31">
-        <v>0.5957003351452458</v>
+        <v>0.6029507070293678</v>
       </c>
       <c r="L31">
         <v>2</v>
@@ -2010,37 +2022,37 @@
         <v>43</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>2024</v>
       </c>
       <c r="F32">
-        <v>0.590909</v>
+        <v>0.318182</v>
       </c>
       <c r="G32">
-        <v>0.574949</v>
+        <v>0.461864</v>
       </c>
       <c r="H32">
-        <v>0.530803</v>
+        <v>0.498498</v>
       </c>
       <c r="I32">
-        <v>0.472222</v>
+        <v>0.263158</v>
       </c>
       <c r="J32">
-        <v>0.5235340000000001</v>
+        <v>0.506526</v>
       </c>
       <c r="K32">
-        <v>0.5530765276973424</v>
+        <v>0.3777255699150836</v>
       </c>
       <c r="L32">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -2051,37 +2063,37 @@
         <v>44</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E33">
         <v>2024</v>
       </c>
       <c r="F33">
-        <v>0.590909</v>
+        <v>0.263158</v>
       </c>
       <c r="G33">
-        <v>0.581109</v>
+        <v>0.518987</v>
       </c>
       <c r="H33">
-        <v>0.54123</v>
+        <v>0.471608</v>
       </c>
       <c r="I33">
-        <v>0.45993</v>
+        <v>0.323232</v>
       </c>
       <c r="J33">
-        <v>0.5374</v>
+        <v>0.425725</v>
       </c>
       <c r="K33">
-        <v>0.5554073330774769</v>
+        <v>0.3801415478167181</v>
       </c>
       <c r="L33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -2095,37 +2107,37 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E34">
         <v>2024</v>
       </c>
       <c r="F34">
-        <v>0.285714</v>
+        <v>0.590909</v>
       </c>
       <c r="G34">
-        <v>0.449679</v>
+        <v>0.574949</v>
       </c>
       <c r="H34">
-        <v>0.473515</v>
+        <v>0.530803</v>
       </c>
       <c r="I34">
-        <v>0.140625</v>
+        <v>0.472222</v>
       </c>
       <c r="J34">
-        <v>0.504463</v>
+        <v>0.5235340000000001</v>
       </c>
       <c r="K34">
-        <v>0.3515430719859096</v>
+        <v>0.5579002325129716</v>
       </c>
       <c r="L34">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2136,37 +2148,37 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <v>2024</v>
       </c>
       <c r="F35">
-        <v>0.227273</v>
+        <v>0.590909</v>
       </c>
       <c r="G35">
-        <v>0.471429</v>
+        <v>0.581109</v>
       </c>
       <c r="H35">
-        <v>0.494575</v>
+        <v>0.54123</v>
       </c>
       <c r="I35">
-        <v>0.210526</v>
+        <v>0.45993</v>
       </c>
       <c r="J35">
-        <v>0.482828</v>
+        <v>0.5374</v>
       </c>
       <c r="K35">
-        <v>0.3476815708603639</v>
+        <v>0.5592599618742015</v>
       </c>
       <c r="L35">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2177,34 +2189,34 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>2024</v>
+      </c>
+      <c r="F36">
+        <v>0.285714</v>
+      </c>
+      <c r="G36">
+        <v>0.449679</v>
+      </c>
+      <c r="H36">
+        <v>0.473515</v>
+      </c>
+      <c r="I36">
+        <v>0.140625</v>
+      </c>
+      <c r="J36">
+        <v>0.504463</v>
+      </c>
+      <c r="K36">
+        <v>0.3393541350115772</v>
+      </c>
+      <c r="L36">
         <v>9</v>
-      </c>
-      <c r="E36">
-        <v>2024</v>
-      </c>
-      <c r="F36">
-        <v>0.173913</v>
-      </c>
-      <c r="G36">
-        <v>0.575937</v>
-      </c>
-      <c r="H36">
-        <v>0.482784</v>
-      </c>
-      <c r="I36">
-        <v>0.264368</v>
-      </c>
-      <c r="J36">
-        <v>0.516393</v>
-      </c>
-      <c r="K36">
-        <v>0.3745519342913954</v>
-      </c>
-      <c r="L36">
-        <v>7</v>
       </c>
       <c r="M36">
         <v>2</v>
@@ -2218,34 +2230,34 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>2024</v>
+      </c>
+      <c r="F37">
+        <v>0.227273</v>
+      </c>
+      <c r="G37">
+        <v>0.471429</v>
+      </c>
+      <c r="H37">
+        <v>0.494575</v>
+      </c>
+      <c r="I37">
+        <v>0.210526</v>
+      </c>
+      <c r="J37">
+        <v>0.482828</v>
+      </c>
+      <c r="K37">
+        <v>0.3356914316385797</v>
+      </c>
+      <c r="L37">
         <v>10</v>
-      </c>
-      <c r="E37">
-        <v>2024</v>
-      </c>
-      <c r="F37">
-        <v>0.136364</v>
-      </c>
-      <c r="G37">
-        <v>0.549696</v>
-      </c>
-      <c r="H37">
-        <v>0.514426</v>
-      </c>
-      <c r="I37">
-        <v>0.294118</v>
-      </c>
-      <c r="J37">
-        <v>0.487162</v>
-      </c>
-      <c r="K37">
-        <v>0.3559485614141077</v>
-      </c>
-      <c r="L37">
-        <v>8</v>
       </c>
       <c r="M37">
         <v>2</v>
@@ -2259,34 +2271,34 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D38">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>2024</v>
+      </c>
+      <c r="F38">
+        <v>0.173913</v>
+      </c>
+      <c r="G38">
+        <v>0.575937</v>
+      </c>
+      <c r="H38">
+        <v>0.482784</v>
+      </c>
+      <c r="I38">
+        <v>0.264368</v>
+      </c>
+      <c r="J38">
+        <v>0.516393</v>
+      </c>
+      <c r="K38">
+        <v>0.3642625130474204</v>
+      </c>
+      <c r="L38">
         <v>7</v>
-      </c>
-      <c r="E38">
-        <v>2024</v>
-      </c>
-      <c r="F38">
-        <v>0.318182</v>
-      </c>
-      <c r="G38">
-        <v>0.452229</v>
-      </c>
-      <c r="H38">
-        <v>0.495644</v>
-      </c>
-      <c r="I38">
-        <v>0.222222</v>
-      </c>
-      <c r="J38">
-        <v>0.453543</v>
-      </c>
-      <c r="K38">
-        <v>0.3700884320276229</v>
-      </c>
-      <c r="L38">
-        <v>9</v>
       </c>
       <c r="M38">
         <v>2</v>
@@ -2300,34 +2312,34 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D39">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E39">
         <v>2024</v>
       </c>
       <c r="F39">
-        <v>0.090909</v>
+        <v>0.136364</v>
       </c>
       <c r="G39">
-        <v>0.583682</v>
+        <v>0.549696</v>
       </c>
       <c r="H39">
-        <v>0.476707</v>
+        <v>0.514426</v>
       </c>
       <c r="I39">
-        <v>0.477273</v>
+        <v>0.294118</v>
       </c>
       <c r="J39">
-        <v>0.472222</v>
+        <v>0.487162</v>
       </c>
       <c r="K39">
-        <v>0.3778826566395957</v>
+        <v>0.3441865259336299</v>
       </c>
       <c r="L39">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M39">
         <v>2</v>
@@ -2341,37 +2353,37 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E40">
         <v>2024</v>
       </c>
       <c r="F40">
-        <v>0.545455</v>
+        <v>0.318182</v>
       </c>
       <c r="G40">
-        <v>0.56341</v>
+        <v>0.452229</v>
       </c>
       <c r="H40">
-        <v>0.510672</v>
+        <v>0.495644</v>
       </c>
       <c r="I40">
-        <v>0.433962</v>
+        <v>0.222222</v>
       </c>
       <c r="J40">
-        <v>0.498773</v>
+        <v>0.453543</v>
       </c>
       <c r="K40">
-        <v>0.523170549216883</v>
+        <v>0.3626134433133498</v>
       </c>
       <c r="L40">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2382,37 +2394,37 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D41">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E41">
         <v>2024</v>
       </c>
       <c r="F41">
-        <v>0.619048</v>
+        <v>0.090909</v>
       </c>
       <c r="G41">
-        <v>0.490196</v>
+        <v>0.583682</v>
       </c>
       <c r="H41">
-        <v>0.501389</v>
+        <v>0.476707</v>
       </c>
       <c r="I41">
-        <v>0.380783</v>
+        <v>0.477273</v>
       </c>
       <c r="J41">
-        <v>0.49124</v>
+        <v>0.472222</v>
       </c>
       <c r="K41">
-        <v>0.5156713274038485</v>
+        <v>0.3690965011104564</v>
       </c>
       <c r="L41">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2423,37 +2435,37 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42">
         <v>2024</v>
       </c>
       <c r="F42">
-        <v>0.619048</v>
+        <v>0.545455</v>
       </c>
       <c r="G42">
-        <v>0.514161</v>
+        <v>0.56341</v>
       </c>
       <c r="H42">
-        <v>0.546207</v>
+        <v>0.510672</v>
       </c>
       <c r="I42">
-        <v>0.348592</v>
+        <v>0.433962</v>
       </c>
       <c r="J42">
-        <v>0.558577</v>
+        <v>0.498773</v>
       </c>
       <c r="K42">
-        <v>0.5296471349362624</v>
+        <v>0.5277107390915369</v>
       </c>
       <c r="L42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2464,34 +2476,34 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E43">
         <v>2024</v>
       </c>
       <c r="F43">
-        <v>0.318182</v>
+        <v>0.619048</v>
       </c>
       <c r="G43">
-        <v>0.480932</v>
+        <v>0.490196</v>
       </c>
       <c r="H43">
-        <v>0.486419</v>
+        <v>0.501389</v>
       </c>
       <c r="I43">
-        <v>0.267123</v>
+        <v>0.380783</v>
       </c>
       <c r="J43">
-        <v>0.498878</v>
+        <v>0.49124</v>
       </c>
       <c r="K43">
-        <v>0.3928706046449029</v>
+        <v>0.5196808311375287</v>
       </c>
       <c r="L43">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M43">
         <v>1</v>
@@ -2505,37 +2517,37 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D44">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E44">
         <v>2024</v>
       </c>
       <c r="F44">
-        <v>0.272727</v>
+        <v>0.619048</v>
       </c>
       <c r="G44">
-        <v>0.552361</v>
+        <v>0.514161</v>
       </c>
       <c r="H44">
-        <v>0.490404</v>
+        <v>0.546207</v>
       </c>
       <c r="I44">
-        <v>0.305344</v>
+        <v>0.348592</v>
       </c>
       <c r="J44">
-        <v>0.479898</v>
+        <v>0.558577</v>
       </c>
       <c r="K44">
-        <v>0.4024428047059267</v>
+        <v>0.5289168610360282</v>
       </c>
       <c r="L44">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2546,10 +2558,10 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E45">
         <v>2024</v>
@@ -2558,22 +2570,22 @@
         <v>0.318182</v>
       </c>
       <c r="G45">
-        <v>0.609053</v>
+        <v>0.480932</v>
       </c>
       <c r="H45">
-        <v>0.526678</v>
+        <v>0.486419</v>
       </c>
       <c r="I45">
-        <v>0.496732</v>
+        <v>0.267123</v>
       </c>
       <c r="J45">
-        <v>0.500455</v>
+        <v>0.498878</v>
       </c>
       <c r="K45">
-        <v>0.4717282958608465</v>
+        <v>0.3842278339435934</v>
       </c>
       <c r="L45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M45">
         <v>1</v>
@@ -2587,34 +2599,34 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <v>2024</v>
+      </c>
+      <c r="F46">
+        <v>0.272727</v>
+      </c>
+      <c r="G46">
+        <v>0.552361</v>
+      </c>
+      <c r="H46">
+        <v>0.490404</v>
+      </c>
+      <c r="I46">
+        <v>0.305344</v>
+      </c>
+      <c r="J46">
+        <v>0.479898</v>
+      </c>
+      <c r="K46">
+        <v>0.3972107129654874</v>
+      </c>
+      <c r="L46">
         <v>7</v>
-      </c>
-      <c r="E46">
-        <v>2024</v>
-      </c>
-      <c r="F46">
-        <v>0.47619</v>
-      </c>
-      <c r="G46">
-        <v>0.549654</v>
-      </c>
-      <c r="H46">
-        <v>0.495572</v>
-      </c>
-      <c r="I46">
-        <v>0.362694</v>
-      </c>
-      <c r="J46">
-        <v>0.510305</v>
-      </c>
-      <c r="K46">
-        <v>0.4848356629425897</v>
-      </c>
-      <c r="L46">
-        <v>6</v>
       </c>
       <c r="M46">
         <v>1</v>
@@ -2628,34 +2640,34 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D47">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E47">
         <v>2024</v>
       </c>
       <c r="F47">
-        <v>0.454545</v>
+        <v>0.318182</v>
       </c>
       <c r="G47">
-        <v>0.519751</v>
+        <v>0.609053</v>
       </c>
       <c r="H47">
-        <v>0.536392</v>
+        <v>0.526678</v>
       </c>
       <c r="I47">
-        <v>0.345622</v>
+        <v>0.496732</v>
       </c>
       <c r="J47">
-        <v>0.537889</v>
+        <v>0.500455</v>
       </c>
       <c r="K47">
-        <v>0.4717695335361308</v>
+        <v>0.469767090225821</v>
       </c>
       <c r="L47">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -2669,34 +2681,34 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D48">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E48">
         <v>2024</v>
       </c>
       <c r="F48">
-        <v>0.52381</v>
+        <v>0.47619</v>
       </c>
       <c r="G48">
-        <v>0.495614</v>
+        <v>0.549654</v>
       </c>
       <c r="H48">
-        <v>0.527232</v>
+        <v>0.495572</v>
       </c>
       <c r="I48">
-        <v>0.341772</v>
+        <v>0.362694</v>
       </c>
       <c r="J48">
-        <v>0.5197349999999999</v>
+        <v>0.510305</v>
       </c>
       <c r="K48">
-        <v>0.4840874695467475</v>
+        <v>0.4852620444788073</v>
       </c>
       <c r="L48">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -2710,34 +2722,34 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E49">
         <v>2024</v>
       </c>
       <c r="F49">
-        <v>0.47619</v>
+        <v>0.454545</v>
       </c>
       <c r="G49">
-        <v>0.425676</v>
+        <v>0.519751</v>
       </c>
       <c r="H49">
-        <v>0.466042</v>
+        <v>0.536392</v>
       </c>
       <c r="I49">
-        <v>0.266667</v>
+        <v>0.345622</v>
       </c>
       <c r="J49">
-        <v>0.417243</v>
+        <v>0.537889</v>
       </c>
       <c r="K49">
-        <v>0.4160998440726009</v>
+        <v>0.4667346207638389</v>
       </c>
       <c r="L49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M49">
         <v>1</v>
@@ -2751,34 +2763,34 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E50">
         <v>2024</v>
       </c>
       <c r="F50">
-        <v>0.428571</v>
+        <v>0.52381</v>
       </c>
       <c r="G50">
-        <v>0.450116</v>
+        <v>0.495614</v>
       </c>
       <c r="H50">
-        <v>0.485366</v>
+        <v>0.527232</v>
       </c>
       <c r="I50">
-        <v>0.284091</v>
+        <v>0.341772</v>
       </c>
       <c r="J50">
-        <v>0.481328</v>
+        <v>0.5197349999999999</v>
       </c>
       <c r="K50">
-        <v>0.421022115757764</v>
+        <v>0.4819058723438827</v>
       </c>
       <c r="L50">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -2792,7 +2804,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D51">
         <v>4</v>
@@ -2816,7 +2828,7 @@
         <v>0.529213</v>
       </c>
       <c r="K51">
-        <v>0.553069133974871</v>
+        <v>0.5579616442194054</v>
       </c>
       <c r="L51">
         <v>5</v>
@@ -2833,7 +2845,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D52">
         <v>5</v>
@@ -2857,7 +2869,7 @@
         <v>0.528555</v>
       </c>
       <c r="K52">
-        <v>0.5549748412659536</v>
+        <v>0.55979024609343</v>
       </c>
       <c r="L52">
         <v>4</v>
@@ -2874,7 +2886,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D53">
         <v>9</v>
@@ -2898,7 +2910,7 @@
         <v>0.501912</v>
       </c>
       <c r="K53">
-        <v>0.3749561359703368</v>
+        <v>0.3649027593615262</v>
       </c>
       <c r="L53">
         <v>10</v>
@@ -2915,7 +2927,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2939,7 +2951,7 @@
         <v>0.476498</v>
       </c>
       <c r="K54">
-        <v>0.3756592749921086</v>
+        <v>0.3674883349234638</v>
       </c>
       <c r="L54">
         <v>9</v>
@@ -2956,7 +2968,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D55">
         <v>7</v>
@@ -2980,7 +2992,7 @@
         <v>0.469801</v>
       </c>
       <c r="K55">
-        <v>0.4204725131253315</v>
+        <v>0.4179211822047565</v>
       </c>
       <c r="L55">
         <v>8</v>
@@ -2997,7 +3009,7 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D56">
         <v>8</v>
@@ -3021,7 +3033,7 @@
         <v>0.524365</v>
       </c>
       <c r="K56">
-        <v>0.4086973389044395</v>
+        <v>0.3988737033248176</v>
       </c>
       <c r="L56">
         <v>9</v>
@@ -3038,7 +3050,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D57">
         <v>9</v>
@@ -3062,7 +3074,7 @@
         <v>0.523961</v>
       </c>
       <c r="K57">
-        <v>0.4399603361367678</v>
+        <v>0.4344606369110707</v>
       </c>
       <c r="L57">
         <v>7</v>
@@ -3079,7 +3091,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -3103,7 +3115,7 @@
         <v>0.503452</v>
       </c>
       <c r="K58">
-        <v>0.6222214950019699</v>
+        <v>0.6359720682869279</v>
       </c>
       <c r="L58">
         <v>3</v>
@@ -3120,7 +3132,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -3144,7 +3156,7 @@
         <v>0.501038</v>
       </c>
       <c r="K59">
-        <v>0.6263201291110903</v>
+        <v>0.6415320265044284</v>
       </c>
       <c r="L59">
         <v>2</v>
@@ -3161,7 +3173,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D60">
         <v>5</v>
@@ -3185,7 +3197,7 @@
         <v>0.503567</v>
       </c>
       <c r="K60">
-        <v>0.521317878049945</v>
+        <v>0.5258769793092219</v>
       </c>
       <c r="L60">
         <v>6</v>
@@ -3202,7 +3214,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D61">
         <v>6</v>
@@ -3226,7 +3238,7 @@
         <v>0.518728</v>
       </c>
       <c r="K61">
-        <v>0.5259808882733165</v>
+        <v>0.5284421893132327</v>
       </c>
       <c r="L61">
         <v>5</v>
@@ -3243,7 +3255,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D62">
         <v>4</v>
@@ -3267,7 +3279,7 @@
         <v>0.5206769999999999</v>
       </c>
       <c r="K62">
-        <v>0.5146241749804553</v>
+        <v>0.5147764355474305</v>
       </c>
       <c r="L62">
         <v>5</v>
@@ -3284,7 +3296,7 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D63">
         <v>5</v>
@@ -3308,7 +3320,7 @@
         <v>0.523001</v>
       </c>
       <c r="K63">
-        <v>0.5238056181225961</v>
+        <v>0.5263752658087766</v>
       </c>
       <c r="L63">
         <v>4</v>
@@ -3325,7 +3337,7 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D64">
         <v>8</v>
@@ -3349,7 +3361,7 @@
         <v>0.437175</v>
       </c>
       <c r="K64">
-        <v>0.3979202890693734</v>
+        <v>0.3946267253997725</v>
       </c>
       <c r="L64">
         <v>9</v>
@@ -3366,7 +3378,7 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -3390,7 +3402,7 @@
         <v>0.500641</v>
       </c>
       <c r="K65">
-        <v>0.4217806783647149</v>
+        <v>0.4174071366615595</v>
       </c>
       <c r="L65">
         <v>8</v>
@@ -3407,34 +3419,34 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D66">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E66">
         <v>2024</v>
       </c>
       <c r="F66">
-        <v>0.363636</v>
+        <v>0.5</v>
       </c>
       <c r="G66">
-        <v>0.515991</v>
+        <v>0.507853</v>
       </c>
       <c r="H66">
-        <v>0.505158</v>
+        <v>0.496646</v>
       </c>
       <c r="I66">
-        <v>0.242424</v>
+        <v>0.333333</v>
       </c>
       <c r="J66">
-        <v>0.501997</v>
+        <v>0.507155</v>
       </c>
       <c r="K66">
-        <v>0.4156553789180943</v>
+        <v>0.4742224091902126</v>
       </c>
       <c r="L66">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M66">
         <v>1</v>
@@ -3448,34 +3460,34 @@
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E67">
         <v>2024</v>
       </c>
       <c r="F67">
-        <v>0.272727</v>
+        <v>0.619048</v>
       </c>
       <c r="G67">
-        <v>0.567511</v>
+        <v>0.424107</v>
       </c>
       <c r="H67">
-        <v>0.492281</v>
+        <v>0.46689</v>
       </c>
       <c r="I67">
-        <v>0.409449</v>
+        <v>0.29304</v>
       </c>
       <c r="J67">
-        <v>0.469844</v>
+        <v>0.441218</v>
       </c>
       <c r="K67">
-        <v>0.4231071079817842</v>
+        <v>0.4764645704001294</v>
       </c>
       <c r="L67">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M67">
         <v>1</v>
@@ -3489,34 +3501,34 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E68">
         <v>2024</v>
       </c>
       <c r="F68">
-        <v>0.375</v>
+        <v>0.363636</v>
       </c>
       <c r="G68">
-        <v>0.481707</v>
+        <v>0.515991</v>
       </c>
       <c r="H68">
-        <v>0.449171</v>
+        <v>0.505158</v>
       </c>
       <c r="I68">
-        <v>0.176471</v>
+        <v>0.242424</v>
       </c>
       <c r="J68">
-        <v>0.500308</v>
+        <v>0.501997</v>
       </c>
       <c r="K68">
-        <v>0.3955327069368888</v>
+        <v>0.4097552046333527</v>
       </c>
       <c r="L68">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M68">
         <v>1</v>
@@ -3530,34 +3542,34 @@
         <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D69">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E69">
         <v>2024</v>
       </c>
       <c r="F69">
-        <v>0.227273</v>
+        <v>0.272727</v>
       </c>
       <c r="G69">
-        <v>0.584551</v>
+        <v>0.567511</v>
       </c>
       <c r="H69">
-        <v>0.499798</v>
+        <v>0.492281</v>
       </c>
       <c r="I69">
-        <v>0.407407</v>
+        <v>0.409449</v>
       </c>
       <c r="J69">
-        <v>0.480034</v>
+        <v>0.469844</v>
       </c>
       <c r="K69">
-        <v>0.4144001435009697</v>
+        <v>0.419827576348337</v>
       </c>
       <c r="L69">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M69">
         <v>1</v>
@@ -3571,37 +3583,37 @@
         <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D70">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E70">
         <v>2024</v>
       </c>
       <c r="F70">
-        <v>0.454545</v>
+        <v>0.375</v>
       </c>
       <c r="G70">
-        <v>0.416136</v>
+        <v>0.481707</v>
       </c>
       <c r="H70">
-        <v>0.465626</v>
+        <v>0.449171</v>
       </c>
       <c r="I70">
-        <v>0.229665</v>
+        <v>0.176471</v>
       </c>
       <c r="J70">
-        <v>0.456952</v>
+        <v>0.500308</v>
       </c>
       <c r="K70">
-        <v>0.4058547405788994</v>
+        <v>0.3895333751855221</v>
       </c>
       <c r="L70">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M70">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -3612,34 +3624,34 @@
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D71">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E71">
         <v>2024</v>
       </c>
       <c r="F71">
-        <v>0.409091</v>
+        <v>0.227273</v>
       </c>
       <c r="G71">
-        <v>0.471698</v>
+        <v>0.584551</v>
       </c>
       <c r="H71">
-        <v>0.501599</v>
+        <v>0.499798</v>
       </c>
       <c r="I71">
-        <v>0.21134</v>
+        <v>0.407407</v>
       </c>
       <c r="J71">
-        <v>0.481152</v>
+        <v>0.480034</v>
       </c>
       <c r="K71">
-        <v>0.4091735112200843</v>
+        <v>0.4093683384680432</v>
       </c>
       <c r="L71">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M71">
         <v>1</v>
@@ -3653,31 +3665,31 @@
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E72">
         <v>2024</v>
       </c>
       <c r="F72">
-        <v>0.45</v>
+        <v>0.454545</v>
       </c>
       <c r="G72">
-        <v>0.436725</v>
+        <v>0.416136</v>
       </c>
       <c r="H72">
-        <v>0.459671</v>
+        <v>0.465626</v>
       </c>
       <c r="I72">
-        <v>0.175439</v>
+        <v>0.229665</v>
       </c>
       <c r="J72">
-        <v>0.49484</v>
+        <v>0.456952</v>
       </c>
       <c r="K72">
-        <v>0.4068692771269851</v>
+        <v>0.4022767440531584</v>
       </c>
       <c r="L72">
         <v>9</v>
@@ -3694,34 +3706,34 @@
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D73">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E73">
         <v>2024</v>
       </c>
       <c r="F73">
-        <v>0.318182</v>
+        <v>0.409091</v>
       </c>
       <c r="G73">
-        <v>0.423077</v>
+        <v>0.471698</v>
       </c>
       <c r="H73">
-        <v>0.45305</v>
+        <v>0.501599</v>
       </c>
       <c r="I73">
-        <v>0.174825</v>
+        <v>0.21134</v>
       </c>
       <c r="J73">
-        <v>0.468866</v>
+        <v>0.481152</v>
       </c>
       <c r="K73">
-        <v>0.3540077279844012</v>
+        <v>0.4040661471690283</v>
       </c>
       <c r="L73">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="M73">
         <v>1</v>
@@ -3735,34 +3747,34 @@
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>2024</v>
+      </c>
+      <c r="F74">
+        <v>0.318182</v>
+      </c>
+      <c r="G74">
+        <v>0.423077</v>
+      </c>
+      <c r="H74">
+        <v>0.45305</v>
+      </c>
+      <c r="I74">
+        <v>0.174825</v>
+      </c>
+      <c r="J74">
+        <v>0.468866</v>
+      </c>
+      <c r="K74">
+        <v>0.3448309652170864</v>
+      </c>
+      <c r="L74">
         <v>13</v>
-      </c>
-      <c r="E74">
-        <v>2024</v>
-      </c>
-      <c r="F74">
-        <v>0.263158</v>
-      </c>
-      <c r="G74">
-        <v>0.498708</v>
-      </c>
-      <c r="H74">
-        <v>0.452902</v>
-      </c>
-      <c r="I74">
-        <v>0.152174</v>
-      </c>
-      <c r="J74">
-        <v>0.5142600000000001</v>
-      </c>
-      <c r="K74">
-        <v>0.3611050186953324</v>
-      </c>
-      <c r="L74">
-        <v>12</v>
       </c>
       <c r="M74">
         <v>1</v>
@@ -3776,34 +3788,34 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E75">
         <v>2024</v>
       </c>
       <c r="F75">
-        <v>0.318182</v>
+        <v>0.263158</v>
       </c>
       <c r="G75">
-        <v>0.493724</v>
+        <v>0.498708</v>
       </c>
       <c r="H75">
-        <v>0.506964</v>
+        <v>0.452902</v>
       </c>
       <c r="I75">
-        <v>0.264901</v>
+        <v>0.152174</v>
       </c>
       <c r="J75">
-        <v>0.498385</v>
+        <v>0.5142600000000001</v>
       </c>
       <c r="K75">
-        <v>0.3970680952223845</v>
+        <v>0.3505496978395991</v>
       </c>
       <c r="L75">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M75">
         <v>1</v>
@@ -3817,31 +3829,31 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D76">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E76">
         <v>2024</v>
       </c>
       <c r="F76">
-        <v>0.45</v>
+        <v>0.333333</v>
       </c>
       <c r="G76">
-        <v>0.401985</v>
+        <v>0.480349</v>
       </c>
       <c r="H76">
-        <v>0.457106</v>
+        <v>0.508821</v>
       </c>
       <c r="I76">
-        <v>0.236994</v>
+        <v>0.291391</v>
       </c>
       <c r="J76">
-        <v>0.45097</v>
+        <v>0.491504</v>
       </c>
       <c r="K76">
-        <v>0.400085665186207</v>
+        <v>0.3936504839658229</v>
       </c>
       <c r="L76">
         <v>10</v>
@@ -3858,34 +3870,34 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D77">
+        <v>10</v>
+      </c>
+      <c r="E77">
+        <v>2024</v>
+      </c>
+      <c r="F77">
+        <v>0.318182</v>
+      </c>
+      <c r="G77">
+        <v>0.493724</v>
+      </c>
+      <c r="H77">
+        <v>0.506964</v>
+      </c>
+      <c r="I77">
+        <v>0.264901</v>
+      </c>
+      <c r="J77">
+        <v>0.498385</v>
+      </c>
+      <c r="K77">
+        <v>0.3885790348152788</v>
+      </c>
+      <c r="L77">
         <v>11</v>
-      </c>
-      <c r="E77">
-        <v>2024</v>
-      </c>
-      <c r="F77">
-        <v>0.35</v>
-      </c>
-      <c r="G77">
-        <v>0.47494</v>
-      </c>
-      <c r="H77">
-        <v>0.494839</v>
-      </c>
-      <c r="I77">
-        <v>0.148148</v>
-      </c>
-      <c r="J77">
-        <v>0.488326</v>
-      </c>
-      <c r="K77">
-        <v>0.3803470843068538</v>
-      </c>
-      <c r="L77">
-        <v>12</v>
       </c>
       <c r="M77">
         <v>1</v>
@@ -3899,37 +3911,37 @@
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D78">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E78">
         <v>2024</v>
       </c>
       <c r="F78">
-        <v>0.272727</v>
+        <v>0.45</v>
       </c>
       <c r="G78">
-        <v>0.516807</v>
+        <v>0.401985</v>
       </c>
       <c r="H78">
-        <v>0.487914</v>
+        <v>0.457106</v>
       </c>
       <c r="I78">
-        <v>0.207692</v>
+        <v>0.236994</v>
       </c>
       <c r="J78">
-        <v>0.496575</v>
+        <v>0.45097</v>
       </c>
       <c r="K78">
-        <v>0.3778250018779014</v>
+        <v>0.3962660157091454</v>
       </c>
       <c r="L78">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="M78">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -3940,37 +3952,37 @@
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D79">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E79">
         <v>2024</v>
       </c>
       <c r="F79">
-        <v>0.227273</v>
+        <v>0.35</v>
       </c>
       <c r="G79">
-        <v>0.564935</v>
+        <v>0.47494</v>
       </c>
       <c r="H79">
-        <v>0.493645</v>
+        <v>0.494839</v>
       </c>
       <c r="I79">
-        <v>0.257732</v>
+        <v>0.148148</v>
       </c>
       <c r="J79">
-        <v>0.508257</v>
+        <v>0.488326</v>
       </c>
       <c r="K79">
-        <v>0.3873267252209505</v>
+        <v>0.3725275184917464</v>
       </c>
       <c r="L79">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M79">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -3981,34 +3993,34 @@
         <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E80">
         <v>2024</v>
       </c>
       <c r="F80">
-        <v>0.695652</v>
+        <v>0.272727</v>
       </c>
       <c r="G80">
-        <v>0.522634</v>
+        <v>0.516807</v>
       </c>
       <c r="H80">
-        <v>0.479826</v>
+        <v>0.487914</v>
       </c>
       <c r="I80">
-        <v>0.431138</v>
+        <v>0.207692</v>
       </c>
       <c r="J80">
-        <v>0.482194</v>
+        <v>0.496575</v>
       </c>
       <c r="K80">
-        <v>0.5573278777355385</v>
+        <v>0.3691592881737207</v>
       </c>
       <c r="L80">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="M80">
         <v>1</v>
@@ -4022,37 +4034,37 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D81">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E81">
         <v>2024</v>
       </c>
       <c r="F81">
-        <v>0.782609</v>
+        <v>0.227273</v>
       </c>
       <c r="G81">
-        <v>0.449597</v>
+        <v>0.564935</v>
       </c>
       <c r="H81">
-        <v>0.502911</v>
+        <v>0.493645</v>
       </c>
       <c r="I81">
-        <v>0.362694</v>
+        <v>0.257732</v>
       </c>
       <c r="J81">
-        <v>0.5084379999999999</v>
+        <v>0.508257</v>
       </c>
       <c r="K81">
-        <v>0.5583902908854417</v>
+        <v>0.3787394708505832</v>
       </c>
       <c r="L81">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M81">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -4063,7 +4075,7 @@
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D82">
         <v>10</v>
@@ -4087,7 +4099,7 @@
         <v>0.494718</v>
       </c>
       <c r="K82">
-        <v>0.4322773836663079</v>
+        <v>0.428587073548531</v>
       </c>
       <c r="L82">
         <v>11</v>
@@ -4104,7 +4116,7 @@
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D83">
         <v>11</v>
@@ -4128,7 +4140,7 @@
         <v>0.508954</v>
       </c>
       <c r="K83">
-        <v>0.4398228807816009</v>
+        <v>0.4369949144323977</v>
       </c>
       <c r="L83">
         <v>10</v>
@@ -4145,7 +4157,7 @@
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -4169,7 +4181,7 @@
         <v>0.493517</v>
       </c>
       <c r="K84">
-        <v>0.5783973275461064</v>
+        <v>0.5877156498489702</v>
       </c>
       <c r="L84">
         <v>4</v>
@@ -4186,37 +4198,37 @@
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D85">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E85">
         <v>2024</v>
       </c>
       <c r="F85">
-        <v>0.7727270000000001</v>
+        <v>0.714286</v>
       </c>
       <c r="G85">
-        <v>0.509514</v>
+        <v>0.566372</v>
       </c>
       <c r="H85">
-        <v>0.496277</v>
+        <v>0.500254</v>
       </c>
       <c r="I85">
-        <v>0.436813</v>
+        <v>0.454829</v>
       </c>
       <c r="J85">
-        <v>0.508107</v>
+        <v>0.501481</v>
       </c>
       <c r="K85">
-        <v>0.5850714292873055</v>
+        <v>0.5957635262861941</v>
       </c>
       <c r="L85">
         <v>2</v>
       </c>
       <c r="M85">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -4227,34 +4239,34 @@
         <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D86">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E86">
         <v>2024</v>
       </c>
       <c r="F86">
-        <v>0.6</v>
+        <v>0.7727270000000001</v>
       </c>
       <c r="G86">
-        <v>0.434988</v>
+        <v>0.509514</v>
       </c>
       <c r="H86">
-        <v>0.512981</v>
+        <v>0.496277</v>
       </c>
       <c r="I86">
-        <v>0.309524</v>
+        <v>0.436813</v>
       </c>
       <c r="J86">
-        <v>0.506314</v>
+        <v>0.508107</v>
       </c>
       <c r="K86">
-        <v>0.4836238012268299</v>
+        <v>0.5951975617435772</v>
       </c>
       <c r="L86">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M86">
         <v>1</v>
@@ -4268,34 +4280,34 @@
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D87">
+        <v>6</v>
+      </c>
+      <c r="E87">
+        <v>2024</v>
+      </c>
+      <c r="F87">
+        <v>0.6</v>
+      </c>
+      <c r="G87">
+        <v>0.434988</v>
+      </c>
+      <c r="H87">
+        <v>0.512981</v>
+      </c>
+      <c r="I87">
+        <v>0.309524</v>
+      </c>
+      <c r="J87">
+        <v>0.506314</v>
+      </c>
+      <c r="K87">
+        <v>0.4823120266259441</v>
+      </c>
+      <c r="L87">
         <v>7</v>
-      </c>
-      <c r="E87">
-        <v>2024</v>
-      </c>
-      <c r="F87">
-        <v>0.454545</v>
-      </c>
-      <c r="G87">
-        <v>0.572043</v>
-      </c>
-      <c r="H87">
-        <v>0.499488</v>
-      </c>
-      <c r="I87">
-        <v>0.35122</v>
-      </c>
-      <c r="J87">
-        <v>0.532826</v>
-      </c>
-      <c r="K87">
-        <v>0.4858997244867889</v>
-      </c>
-      <c r="L87">
-        <v>6</v>
       </c>
       <c r="M87">
         <v>1</v>
@@ -4309,34 +4321,34 @@
         <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D88">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E88">
         <v>2024</v>
       </c>
       <c r="F88">
-        <v>0.35</v>
+        <v>0.454545</v>
       </c>
       <c r="G88">
-        <v>0.446602</v>
+        <v>0.572043</v>
       </c>
       <c r="H88">
-        <v>0.487883</v>
+        <v>0.499488</v>
       </c>
       <c r="I88">
-        <v>0.211679</v>
+        <v>0.35122</v>
       </c>
       <c r="J88">
-        <v>0.526215</v>
+        <v>0.532826</v>
       </c>
       <c r="K88">
-        <v>0.388311351304627</v>
+        <v>0.4849575878185668</v>
       </c>
       <c r="L88">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M88">
         <v>1</v>
@@ -4350,34 +4362,34 @@
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D89">
+        <v>11</v>
+      </c>
+      <c r="E89">
+        <v>2024</v>
+      </c>
+      <c r="F89">
+        <v>0.35</v>
+      </c>
+      <c r="G89">
+        <v>0.446602</v>
+      </c>
+      <c r="H89">
+        <v>0.487883</v>
+      </c>
+      <c r="I89">
+        <v>0.211679</v>
+      </c>
+      <c r="J89">
+        <v>0.526215</v>
+      </c>
+      <c r="K89">
+        <v>0.3768781385844684</v>
+      </c>
+      <c r="L89">
         <v>12</v>
-      </c>
-      <c r="E89">
-        <v>2024</v>
-      </c>
-      <c r="F89">
-        <v>0.318182</v>
-      </c>
-      <c r="G89">
-        <v>0.510684</v>
-      </c>
-      <c r="H89">
-        <v>0.5</v>
-      </c>
-      <c r="I89">
-        <v>0.202797</v>
-      </c>
-      <c r="J89">
-        <v>0.513283</v>
-      </c>
-      <c r="K89">
-        <v>0.3935887889740814</v>
-      </c>
-      <c r="L89">
-        <v>11</v>
       </c>
       <c r="M89">
         <v>1</v>
@@ -4391,34 +4403,34 @@
         <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D90">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E90">
         <v>2024</v>
       </c>
       <c r="F90">
-        <v>0.238095</v>
+        <v>0.318182</v>
       </c>
       <c r="G90">
-        <v>0.478555</v>
+        <v>0.510684</v>
       </c>
       <c r="H90">
-        <v>0.511857</v>
+        <v>0.5</v>
       </c>
       <c r="I90">
-        <v>0.153846</v>
+        <v>0.202797</v>
       </c>
       <c r="J90">
-        <v>0.540909</v>
+        <v>0.513283</v>
       </c>
       <c r="K90">
-        <v>0.3535692956112804</v>
+        <v>0.3848369292147701</v>
       </c>
       <c r="L90">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M90">
         <v>1</v>
@@ -4432,34 +4444,34 @@
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D91">
+        <v>13</v>
+      </c>
+      <c r="E91">
+        <v>2024</v>
+      </c>
+      <c r="F91">
+        <v>0.238095</v>
+      </c>
+      <c r="G91">
+        <v>0.478555</v>
+      </c>
+      <c r="H91">
+        <v>0.511857</v>
+      </c>
+      <c r="I91">
+        <v>0.153846</v>
+      </c>
+      <c r="J91">
+        <v>0.540909</v>
+      </c>
+      <c r="K91">
+        <v>0.3376134211154045</v>
+      </c>
+      <c r="L91">
         <v>14</v>
-      </c>
-      <c r="E91">
-        <v>2024</v>
-      </c>
-      <c r="F91">
-        <v>0.136364</v>
-      </c>
-      <c r="G91">
-        <v>0.52452</v>
-      </c>
-      <c r="H91">
-        <v>0.5073220000000001</v>
-      </c>
-      <c r="I91">
-        <v>0.435484</v>
-      </c>
-      <c r="J91">
-        <v>0.46717</v>
-      </c>
-      <c r="K91">
-        <v>0.3690548424109409</v>
-      </c>
-      <c r="L91">
-        <v>13</v>
       </c>
       <c r="M91">
         <v>1</v>
@@ -4473,34 +4485,34 @@
         <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D92">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E92">
         <v>2024</v>
       </c>
       <c r="F92">
-        <v>0.055556</v>
+        <v>0.136364</v>
       </c>
       <c r="G92">
-        <v>0.501319</v>
+        <v>0.52452</v>
       </c>
       <c r="H92">
-        <v>0.474182</v>
+        <v>0.5073220000000001</v>
       </c>
       <c r="I92">
-        <v>0.058824</v>
+        <v>0.435484</v>
       </c>
       <c r="J92">
-        <v>0.554945</v>
+        <v>0.46717</v>
       </c>
       <c r="K92">
-        <v>0.2833291168653205</v>
+        <v>0.3582365441446406</v>
       </c>
       <c r="L92">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M92">
         <v>1</v>
@@ -4514,34 +4526,34 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D93">
+        <v>15</v>
+      </c>
+      <c r="E93">
+        <v>2024</v>
+      </c>
+      <c r="F93">
+        <v>0.055556</v>
+      </c>
+      <c r="G93">
+        <v>0.501319</v>
+      </c>
+      <c r="H93">
+        <v>0.474182</v>
+      </c>
+      <c r="I93">
+        <v>0.058824</v>
+      </c>
+      <c r="J93">
+        <v>0.554945</v>
+      </c>
+      <c r="K93">
+        <v>0.2611601312981776</v>
+      </c>
+      <c r="L93">
         <v>16</v>
-      </c>
-      <c r="E93">
-        <v>2024</v>
-      </c>
-      <c r="F93">
-        <v>0.045455</v>
-      </c>
-      <c r="G93">
-        <v>0.5629</v>
-      </c>
-      <c r="H93">
-        <v>0.497823</v>
-      </c>
-      <c r="I93">
-        <v>0.136364</v>
-      </c>
-      <c r="J93">
-        <v>0.52452</v>
-      </c>
-      <c r="K93">
-        <v>0.3075998285154815</v>
-      </c>
-      <c r="L93">
-        <v>15</v>
       </c>
       <c r="M93">
         <v>1</v>
@@ -4555,34 +4567,34 @@
         <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D94">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E94">
         <v>2024</v>
       </c>
       <c r="F94">
-        <v>0.272727</v>
+        <v>0.045455</v>
       </c>
       <c r="G94">
-        <v>0.427332</v>
+        <v>0.5629</v>
       </c>
       <c r="H94">
-        <v>0.476893</v>
+        <v>0.497823</v>
       </c>
       <c r="I94">
-        <v>0.177419</v>
+        <v>0.136364</v>
       </c>
       <c r="J94">
-        <v>0.495357</v>
+        <v>0.52452</v>
       </c>
       <c r="K94">
-        <v>0.3455081515504068</v>
+        <v>0.2901408230355615</v>
       </c>
       <c r="L94">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M94">
         <v>1</v>
@@ -4596,34 +4608,34 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D95">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E95">
         <v>2024</v>
       </c>
       <c r="F95">
-        <v>0.090909</v>
+        <v>0.521739</v>
       </c>
       <c r="G95">
-        <v>0.511482</v>
+        <v>0.46748</v>
       </c>
       <c r="H95">
-        <v>0.487666</v>
+        <v>0.491916</v>
       </c>
       <c r="I95">
-        <v>0.47619</v>
+        <v>0.333333</v>
       </c>
       <c r="J95">
-        <v>0.41225</v>
+        <v>0.48455</v>
       </c>
       <c r="K95">
-        <v>0.3474314558513657</v>
+        <v>0.4662633718158063</v>
       </c>
       <c r="L95">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="M95">
         <v>1</v>
@@ -4637,34 +4649,34 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D96">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E96">
         <v>2024</v>
       </c>
       <c r="F96">
-        <v>0.619048</v>
+        <v>0.5</v>
       </c>
       <c r="G96">
-        <v>0.521739</v>
+        <v>0.514223</v>
       </c>
       <c r="H96">
-        <v>0.513736</v>
+        <v>0.469999</v>
       </c>
       <c r="I96">
-        <v>0.35461</v>
+        <v>0.294643</v>
       </c>
       <c r="J96">
-        <v>0.506703</v>
+        <v>0.488306</v>
       </c>
       <c r="K96">
-        <v>0.5235036263605812</v>
+        <v>0.4676606167255473</v>
       </c>
       <c r="L96">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M96">
         <v>1</v>
@@ -4678,34 +4690,34 @@
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D97">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E97">
         <v>2024</v>
       </c>
       <c r="F97">
-        <v>0.764706</v>
+        <v>0.272727</v>
       </c>
       <c r="G97">
-        <v>0.416667</v>
+        <v>0.427332</v>
       </c>
       <c r="H97">
-        <v>0.465715</v>
+        <v>0.476893</v>
       </c>
       <c r="I97">
-        <v>0.316514</v>
+        <v>0.177419</v>
       </c>
       <c r="J97">
-        <v>0.479508</v>
+        <v>0.495357</v>
       </c>
       <c r="K97">
-        <v>0.5287179807902413</v>
+        <v>0.3323733697808623</v>
       </c>
       <c r="L97">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="M97">
         <v>1</v>
@@ -4719,34 +4731,34 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D98">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E98">
         <v>2024</v>
       </c>
       <c r="F98">
-        <v>0.421053</v>
+        <v>0.090909</v>
       </c>
       <c r="G98">
-        <v>0.5482089999999999</v>
+        <v>0.511482</v>
       </c>
       <c r="H98">
-        <v>0.465604</v>
+        <v>0.487666</v>
       </c>
       <c r="I98">
-        <v>0.461538</v>
+        <v>0.47619</v>
       </c>
       <c r="J98">
-        <v>0.464781</v>
+        <v>0.41225</v>
       </c>
       <c r="K98">
-        <v>0.4742772574974705</v>
+        <v>0.3387132635150067</v>
       </c>
       <c r="L98">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M98">
         <v>1</v>
@@ -4760,36 +4772,200 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>2024</v>
+      </c>
+      <c r="F99">
+        <v>0.619048</v>
+      </c>
+      <c r="G99">
+        <v>0.521739</v>
+      </c>
+      <c r="H99">
+        <v>0.513736</v>
+      </c>
+      <c r="I99">
+        <v>0.35461</v>
+      </c>
+      <c r="J99">
+        <v>0.506703</v>
+      </c>
+      <c r="K99">
+        <v>0.5276446688381515</v>
+      </c>
+      <c r="L99">
+        <v>5</v>
+      </c>
+      <c r="M99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>119</v>
+      </c>
+      <c r="D100">
+        <v>4</v>
+      </c>
+      <c r="E100">
+        <v>2024</v>
+      </c>
+      <c r="F100">
+        <v>0.764706</v>
+      </c>
+      <c r="G100">
+        <v>0.416667</v>
+      </c>
+      <c r="H100">
+        <v>0.465715</v>
+      </c>
+      <c r="I100">
+        <v>0.316514</v>
+      </c>
+      <c r="J100">
+        <v>0.479508</v>
+      </c>
+      <c r="K100">
+        <v>0.5358590557835782</v>
+      </c>
+      <c r="L100">
+        <v>3</v>
+      </c>
+      <c r="M100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>119</v>
+      </c>
+      <c r="D101">
+        <v>5</v>
+      </c>
+      <c r="E101">
+        <v>2024</v>
+      </c>
+      <c r="F101">
+        <v>0.7</v>
+      </c>
+      <c r="G101">
+        <v>0.464891</v>
+      </c>
+      <c r="H101">
+        <v>0.461398</v>
+      </c>
+      <c r="I101">
+        <v>0.347518</v>
+      </c>
+      <c r="J101">
+        <v>0.461211</v>
+      </c>
+      <c r="K101">
+        <v>0.5321960102659552</v>
+      </c>
+      <c r="L101">
+        <v>4</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>119</v>
+      </c>
+      <c r="D102">
+        <v>7</v>
+      </c>
+      <c r="E102">
+        <v>2024</v>
+      </c>
+      <c r="F102">
+        <v>0.421053</v>
+      </c>
+      <c r="G102">
+        <v>0.5482089999999999</v>
+      </c>
+      <c r="H102">
+        <v>0.465604</v>
+      </c>
+      <c r="I102">
+        <v>0.461538</v>
+      </c>
+      <c r="J102">
+        <v>0.464781</v>
+      </c>
+      <c r="K102">
+        <v>0.4769495444135124</v>
+      </c>
+      <c r="L102">
         <v>8</v>
       </c>
-      <c r="E99">
-        <v>2024</v>
-      </c>
-      <c r="F99">
+      <c r="M102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
+        <v>119</v>
+      </c>
+      <c r="D103">
+        <v>8</v>
+      </c>
+      <c r="E103">
+        <v>2024</v>
+      </c>
+      <c r="F103">
         <v>0.65</v>
       </c>
-      <c r="G99">
+      <c r="G103">
         <v>0.389535</v>
       </c>
-      <c r="H99">
+      <c r="H103">
         <v>0.489822</v>
       </c>
-      <c r="I99">
+      <c r="I103">
         <v>0.304348</v>
       </c>
-      <c r="J99">
+      <c r="J103">
         <v>0.484242</v>
       </c>
-      <c r="K99">
-        <v>0.4817139110895395</v>
-      </c>
-      <c r="L99">
+      <c r="K103">
+        <v>0.482035370304492</v>
+      </c>
+      <c r="L103">
         <v>7</v>
       </c>
-      <c r="M99">
+      <c r="M103">
         <v>1</v>
       </c>
     </row>

</xml_diff>